<commit_message>
BOM and Pick Place for SMT Assembly
</commit_message>
<xml_diff>
--- a/eagle/Bill of Materials.xlsx
+++ b/eagle/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlauer\Documents\GitHub\robot-actuator-esp32-v8\eagle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874D934-3E3A-4819-B4D5-999EEAE0781D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FCE3C8-E511-4026-93E5-B10C87E64CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{042452C7-4880-43A7-8CF4-773658CBA0E7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>Part</t>
   </si>
@@ -415,6 +415,15 @@
   </si>
   <si>
     <t>It's $4.28 per pack of 100. You need 34 per small actuator.</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>JP2, JP3</t>
   </si>
 </sst>
 </file>
@@ -818,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835C5D6E-4F88-4FC8-8679-9566B7BD0E22}">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -905,7 +914,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>103</v>
@@ -949,6 +958,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -1013,7 +1025,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
         <v>87</v>
@@ -1037,7 +1049,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
         <v>84</v>
@@ -1060,6 +1072,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
       <c r="B14" t="s">
         <v>96</v>
       </c>
@@ -1081,6 +1096,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
       <c r="B15" t="s">
         <v>97</v>
       </c>
@@ -1379,9 +1397,6 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>68</v>
-      </c>
       <c r="B29" t="s">
         <v>45</v>
       </c>
@@ -1465,7 +1480,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
       <c r="B33" t="s">
         <v>67</v>
       </c>
@@ -1486,7 +1504,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
         <v>10</v>
       </c>
@@ -1495,7 +1513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>15</v>
       </c>
@@ -1517,7 +1535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1557,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>105</v>
       </c>
@@ -1560,7 +1578,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>17</v>
       </c>
@@ -1582,7 +1600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>20</v>
       </c>
@@ -1604,7 +1622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>106</v>
       </c>
@@ -1625,7 +1643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>125</v>
       </c>
@@ -1647,7 +1665,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C43" s="5">
         <f>SUM(C3:C42)</f>
         <v>15.206966666666666</v>
@@ -1657,12 +1675,12 @@
         <v>16.265866666666664</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B46" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>116</v>
       </c>
@@ -1683,7 +1701,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>119</v>
       </c>
@@ -1739,8 +1757,12 @@
     <hyperlink ref="F48" r:id="rId31" xr:uid="{FBE06268-8BB2-4F6F-BAB2-B593CEEEF1F5}"/>
     <hyperlink ref="F38" r:id="rId32" xr:uid="{9E7B7476-824A-4509-8219-7FFCB780F10F}"/>
     <hyperlink ref="F42" r:id="rId33" xr:uid="{D166C533-FF6E-4D8F-91F4-BCD1C3A82586}"/>
+    <hyperlink ref="F12" r:id="rId34" xr:uid="{9A34347D-7D1E-49EE-8796-375F948619F1}"/>
+    <hyperlink ref="F14" r:id="rId35" xr:uid="{C4576FD0-CCAC-4B01-A0F6-9BF4AD653BED}"/>
+    <hyperlink ref="F15" r:id="rId36" xr:uid="{90518674-B9D9-4622-994D-310A25563C1A}"/>
+    <hyperlink ref="F13" r:id="rId37" xr:uid="{A5B982B0-8044-4FA3-8921-2B1DB1968ADD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId34"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>